<commit_message>
Project List CSE - A
</commit_message>
<xml_diff>
--- a/Project List CSE-A-6th Sem.xlsx
+++ b/Project List CSE-A-6th Sem.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
   <si>
     <t>ABES Institute of Technology, Ghaziabad</t>
   </si>
@@ -290,6 +290,9 @@
   <si>
     <t>Task Tracker app</t>
   </si>
+  <si>
+    <t>Project No</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +301,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -310,53 +313,76 @@
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -379,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -490,15 +516,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -515,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -523,14 +540,56 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -541,59 +600,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,1032 +834,1162 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B75" sqref="B75"/>
+      <selection pane="topRight" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="92" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="9"/>
+    <col min="1" max="1" width="9.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="92" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="12.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="25" t="s">
+      <c r="D6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
         <v>1</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="16">
         <v>2102900100001</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="27">
+        <v>1</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="8" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
         <v>2</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="16">
         <v>2102900100002</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="26" t="s">
+      <c r="D8" s="27">
+        <v>2</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="9" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
         <v>3</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="16">
         <v>2102900100004</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="26" t="s">
+      <c r="D9" s="27">
+        <v>3</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="10" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
         <v>4</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="16">
         <v>2102900100005</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="26" t="s">
+      <c r="D10" s="27">
+        <v>4</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="11" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="15">
         <v>5</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="16">
         <v>2102900100006</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="26" t="s">
+      <c r="D11" s="27">
+        <v>5</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="12" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A12" s="15">
         <v>6</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="16">
         <v>2102900100007</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="26" t="s">
+      <c r="D12" s="27">
+        <v>6</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="13" spans="1:5" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
         <v>7</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="16">
         <v>2102900100008</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="26" t="s">
+      <c r="D13" s="27">
+        <v>7</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="14" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
         <v>8</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="16">
         <v>2102900100009</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="26" t="s">
+      <c r="D14" s="27">
+        <v>8</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="15" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
         <v>9</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="16">
         <v>2102900100010</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="26" t="s">
+      <c r="D15" s="27">
+        <v>9</v>
+      </c>
+      <c r="E15" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="16" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
         <v>10</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="16">
         <v>2102900100011</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="26" t="s">
+      <c r="D16" s="27">
+        <v>10</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+    <row r="17" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
         <v>11</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="16">
         <v>2102900100012</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="26" t="s">
+      <c r="D17" s="27">
+        <v>1</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+    <row r="18" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
         <v>12</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="16">
         <v>2102900100013</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="26" t="s">
+      <c r="D18" s="27">
+        <v>2</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="19" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
         <v>13</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="16">
         <v>2102900100014</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="26" t="s">
+      <c r="D19" s="27">
+        <v>3</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="20" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
         <v>14</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="16">
         <v>2102900100015</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="26" t="s">
+      <c r="D20" s="27">
+        <v>4</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="21" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
         <v>15</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="16">
         <v>2102900100016</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="26" t="s">
+      <c r="D21" s="27">
+        <v>5</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+    <row r="22" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A22" s="15">
         <v>16</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="16">
         <v>2102900100017</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="26" t="s">
+      <c r="D22" s="27">
+        <v>6</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+    <row r="23" spans="1:5" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="15">
         <v>17</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="16">
         <v>2102900100018</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="26" t="s">
+      <c r="D23" s="27">
+        <v>7</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+    <row r="24" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="15">
         <v>18</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="16">
         <v>2102900100019</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="26" t="s">
+      <c r="D24" s="27">
+        <v>8</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+    <row r="25" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="15">
         <v>19</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="16">
         <v>2102900100021</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="26" t="s">
+      <c r="D25" s="27">
+        <v>9</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+    <row r="26" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="15">
         <v>20</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="16">
         <v>2102900100022</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="26" t="s">
+      <c r="D26" s="27">
+        <v>10</v>
+      </c>
+      <c r="E26" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="27" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="15">
         <v>21</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="16">
         <v>2102900100023</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="26" t="s">
+      <c r="D27" s="27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="28" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="15">
         <v>22</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="16">
         <v>2102900100024</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="26" t="s">
+      <c r="D28" s="27">
+        <v>2</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+    <row r="29" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="15">
         <v>23</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="16">
         <v>2102900100025</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="26" t="s">
+      <c r="D29" s="27">
+        <v>3</v>
+      </c>
+      <c r="E29" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+    <row r="30" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A30" s="15">
         <v>24</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="16">
         <v>2102900100027</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="26" t="s">
+      <c r="D30" s="27">
+        <v>4</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+    <row r="31" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A31" s="15">
         <v>25</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="16">
         <v>2102900100028</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="26" t="s">
+      <c r="D31" s="27">
+        <v>5</v>
+      </c>
+      <c r="E31" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+    <row r="32" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A32" s="15">
         <v>26</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="16">
         <v>2102900100029</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="26" t="s">
+      <c r="D32" s="27">
+        <v>6</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+    <row r="33" spans="1:5" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="15">
         <v>27</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="16">
         <v>2102900100030</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="26" t="s">
+      <c r="D33" s="27">
+        <v>7</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+    <row r="34" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="15">
         <v>28</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="16">
         <v>2102900100031</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="26" t="s">
+      <c r="D34" s="27">
+        <v>8</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+    <row r="35" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="15">
         <v>29</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="16">
         <v>2102900100033</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="26" t="s">
+      <c r="D35" s="27">
+        <v>9</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+    <row r="36" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="15">
         <v>30</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="16">
         <v>2102900100034</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="26" t="s">
+      <c r="D36" s="27">
+        <v>10</v>
+      </c>
+      <c r="E36" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+    <row r="37" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="15">
         <v>31</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="16">
         <v>2102900100035</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="26" t="s">
+      <c r="D37" s="27">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+    <row r="38" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="15">
         <v>32</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="16">
         <v>2102900100036</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="26" t="s">
+      <c r="D38" s="27">
+        <v>2</v>
+      </c>
+      <c r="E38" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+    <row r="39" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="15">
         <v>33</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="16">
         <v>2102900100037</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="26" t="s">
+      <c r="D39" s="27">
+        <v>3</v>
+      </c>
+      <c r="E39" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+    <row r="40" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A40" s="15">
         <v>34</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="16">
         <v>2102900100038</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="26" t="s">
+      <c r="D40" s="27">
+        <v>4</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+    <row r="41" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A41" s="15">
         <v>35</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="16">
         <v>2102900100039</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="26" t="s">
+      <c r="D41" s="27">
+        <v>5</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+    <row r="42" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A42" s="15">
         <v>36</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="16">
         <v>2102900100040</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="26" t="s">
+      <c r="D42" s="27">
+        <v>6</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+    <row r="43" spans="1:5" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="15">
         <v>37</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="16">
         <v>2102900100041</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="23"/>
-      <c r="E43" s="26" t="s">
+      <c r="D43" s="27">
+        <v>7</v>
+      </c>
+      <c r="E43" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+    <row r="44" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="15">
         <v>38</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="16">
         <v>2102900100042</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="23"/>
-      <c r="E44" s="26" t="s">
+      <c r="D44" s="27">
+        <v>8</v>
+      </c>
+      <c r="E44" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+    <row r="45" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="15">
         <v>39</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="16">
         <v>2102900100043</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="26" t="s">
+      <c r="D45" s="27">
+        <v>9</v>
+      </c>
+      <c r="E45" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
+    <row r="46" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="15">
         <v>40</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="16">
         <v>2102900100044</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="26" t="s">
+      <c r="D46" s="27">
+        <v>10</v>
+      </c>
+      <c r="E46" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
+    <row r="47" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="15">
         <v>41</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="16">
         <v>2102900100045</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="26" t="s">
+      <c r="D47" s="27">
+        <v>1</v>
+      </c>
+      <c r="E47" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
+    <row r="48" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="15">
         <v>42</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="16">
         <v>2102900100046</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="26" t="s">
+      <c r="D48" s="27">
+        <v>2</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
+    <row r="49" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="15">
         <v>43</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="16">
         <v>2102900100047</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="26" t="s">
+      <c r="D49" s="27">
+        <v>3</v>
+      </c>
+      <c r="E49" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
+    <row r="50" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A50" s="15">
         <v>44</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="16">
         <v>2102900100048</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="26" t="s">
+      <c r="D50" s="27">
+        <v>4</v>
+      </c>
+      <c r="E50" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A51" s="3">
+    <row r="51" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A51" s="15">
         <v>45</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="16">
         <v>2102900100049</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D51" s="23"/>
-      <c r="E51" s="26" t="s">
+      <c r="D51" s="27">
+        <v>5</v>
+      </c>
+      <c r="E51" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
+    <row r="52" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A52" s="15">
         <v>46</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="16">
         <v>2102900100050</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="26" t="s">
+      <c r="D52" s="27">
+        <v>6</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="3">
+    <row r="53" spans="1:5" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="15">
         <v>47</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="16">
         <v>2102900100051</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D53" s="23"/>
-      <c r="E53" s="26" t="s">
+      <c r="D53" s="27">
+        <v>7</v>
+      </c>
+      <c r="E53" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="3">
+    <row r="54" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="15">
         <v>48</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="16">
         <v>2102900100052</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="26" t="s">
+      <c r="D54" s="27">
+        <v>8</v>
+      </c>
+      <c r="E54" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
+    <row r="55" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="15">
         <v>49</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="16">
         <v>2102900100053</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D55" s="23"/>
-      <c r="E55" s="26" t="s">
+      <c r="D55" s="27">
+        <v>9</v>
+      </c>
+      <c r="E55" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="3">
+    <row r="56" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="15">
         <v>50</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="16">
         <v>2102900100054</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="26" t="s">
+      <c r="D56" s="27">
+        <v>10</v>
+      </c>
+      <c r="E56" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="3">
+    <row r="57" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="15">
         <v>51</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B57" s="16">
         <v>2102900100055</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="23"/>
-      <c r="E57" s="26" t="s">
+      <c r="D57" s="27">
+        <v>1</v>
+      </c>
+      <c r="E57" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
+    <row r="58" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="15">
         <v>52</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" s="16">
         <v>2102900100056</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="23"/>
-      <c r="E58" s="26" t="s">
+      <c r="D58" s="27">
+        <v>2</v>
+      </c>
+      <c r="E58" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
+    <row r="59" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="15">
         <v>53</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" s="16">
         <v>2102900100057</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D59" s="23"/>
-      <c r="E59" s="26" t="s">
+      <c r="D59" s="27">
+        <v>3</v>
+      </c>
+      <c r="E59" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
+    <row r="60" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A60" s="15">
         <v>54</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60" s="16">
         <v>2102900100058</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="26" t="s">
+      <c r="D60" s="27">
+        <v>4</v>
+      </c>
+      <c r="E60" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
+    <row r="61" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A61" s="15">
         <v>55</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61" s="16">
         <v>2102900100059</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D61" s="23"/>
-      <c r="E61" s="26" t="s">
+      <c r="D61" s="27">
+        <v>5</v>
+      </c>
+      <c r="E61" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
+    <row r="62" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A62" s="15">
         <v>56</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62" s="16">
         <v>2202900109003</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D62" s="23"/>
-      <c r="E62" s="26" t="s">
+      <c r="D62" s="27">
+        <v>6</v>
+      </c>
+      <c r="E62" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
+    <row r="63" spans="1:5" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="15">
         <v>57</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="16">
         <v>2202900109004</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D63" s="23"/>
-      <c r="E63" s="26" t="s">
+      <c r="D63" s="27">
+        <v>7</v>
+      </c>
+      <c r="E63" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
+    <row r="64" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="15">
         <v>58</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="16">
         <v>2202900109006</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D64" s="23"/>
-      <c r="E64" s="26" t="s">
+      <c r="D64" s="27">
+        <v>8</v>
+      </c>
+      <c r="E64" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
+    <row r="65" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="15">
         <v>59</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="16">
         <v>2202900109007</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D65" s="23"/>
-      <c r="E65" s="26" t="s">
+      <c r="D65" s="27">
+        <v>9</v>
+      </c>
+      <c r="E65" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="3">
+    <row r="66" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="15">
         <v>60</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66" s="16">
         <v>2202900109008</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D66" s="23"/>
-      <c r="E66" s="26" t="s">
+      <c r="D66" s="27">
+        <v>10</v>
+      </c>
+      <c r="E66" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="3">
+    <row r="67" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="15">
         <v>61</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="16">
         <v>2202900109009</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D67" s="23"/>
-      <c r="E67" s="26" t="s">
+      <c r="D67" s="27">
+        <v>1</v>
+      </c>
+      <c r="E67" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="3">
+    <row r="68" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="15">
         <v>62</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68" s="16">
         <v>2202900109010</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D68" s="24"/>
-      <c r="E68" s="26" t="s">
+      <c r="D68" s="27">
+        <v>2</v>
+      </c>
+      <c r="E68" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="3">
+    <row r="69" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="15">
         <v>63</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="16">
         <v>2202900109015</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D69" s="24"/>
-      <c r="E69" s="26" t="s">
+      <c r="D69" s="27">
+        <v>3</v>
+      </c>
+      <c r="E69" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
+    <row r="70" spans="1:5" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A70" s="15">
         <v>64</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B70" s="16">
         <v>2202900109018</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D70" s="24"/>
-      <c r="E70" s="26" t="s">
+      <c r="D70" s="27">
+        <v>4</v>
+      </c>
+      <c r="E70" s="18" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>